<commit_message>
feat: add comment in data before convert using pile
</commit_message>
<xml_diff>
--- a/sample-data/data.xlsx
+++ b/sample-data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/gherkin2tc/sample-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE0ECAC-DC83-A344-B4FE-8BE442B379A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCAF681-38BC-654A-B5FA-14D51F3130E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="37">
   <si>
     <t>code</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>D0006</t>
+  </si>
+  <si>
+    <t># Ini untuk case @P0 @positive @listBuah</t>
+  </si>
+  <si>
+    <t># Ini untuk case @P0 @dataDosen</t>
+  </si>
+  <si>
+    <t># Ini untuk case @P0 @dataDetailDosen</t>
+  </si>
+  <si>
+    <t># Ini untuk case @P0 @joinDataDosen</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -421,696 +433,716 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100000</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>150000</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
+      <c r="A8" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1">
-        <v>12000000</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12000000</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>15000000</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>26</v>
+      <c r="A18" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1">
-        <v>12000000</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12000000</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <v>15000000</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X35" s="1" t="s">
-        <v>26</v>
+      <c r="A35" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="1">
-        <v>12000000</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K36" s="1">
-        <v>12000000</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S36" s="1">
-        <v>12000000</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C37" s="1">
-        <v>15000000</v>
+        <v>12000000</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K37" s="1">
-        <v>15000000</v>
+        <v>12000000</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S37" s="1">
-        <v>15000000</v>
+        <v>12000000</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
-        <v>12000000</v>
+        <v>15000000</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K38" s="1">
-        <v>12000000</v>
+        <v>15000000</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S38" s="1">
-        <v>12000000</v>
+        <v>15000000</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39" s="1">
-        <v>15000000</v>
+        <v>12000000</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K39" s="1">
-        <v>15000000</v>
+        <v>12000000</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="S39" s="1">
-        <v>15000000</v>
+        <v>12000000</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C40" s="1">
-        <v>12000000</v>
+        <v>15000000</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K40" s="1">
-        <v>12000000</v>
+        <v>15000000</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S40" s="1">
-        <v>12000000</v>
+        <v>15000000</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="X40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="1">
+        <v>12000000</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="1">
+        <v>12000000</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S41" s="1">
+        <v>12000000</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C42" s="1">
         <v>15000000</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K42" s="1">
         <v>15000000</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P41" s="1" t="s">
+      <c r="P42" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="Q42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R41" s="1" t="s">
+      <c r="R42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S41" s="1">
+      <c r="S42" s="1">
         <v>15000000</v>
       </c>
-      <c r="T41" s="2" t="s">
+      <c r="T42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U41" s="1" t="s">
+      <c r="U42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V41" s="1" t="s">
+      <c r="V42" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W41" s="1" t="s">
+      <c r="W42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X41" s="1" t="s">
+      <c r="X42" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: tambah guide download-sheet dan finishing download sheet ke excel
</commit_message>
<xml_diff>
--- a/sample-data/data.xlsx
+++ b/sample-data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/gherkin2tc/sample-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCAF681-38BC-654A-B5FA-14D51F3130E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E0A0D5-7E74-5B48-B137-B010F5A7138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="41">
   <si>
     <t>code</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t># Ini untuk case @P0 @joinDataDosen</t>
+  </si>
+  <si>
+    <t>id dosen</t>
+  </si>
+  <si>
+    <t>nama dosen</t>
+  </si>
+  <si>
+    <t>gaji dosen</t>
+  </si>
+  <si>
+    <t>mata kuliah</t>
   </si>
 </sst>
 </file>
@@ -424,7 +436,7 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -477,16 +489,16 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>

</xml_diff>